<commit_message>
Update spec and RTL lib
</commit_message>
<xml_diff>
--- a/input/RegSpec_Org.xlsx
+++ b/input/RegSpec_Org.xlsx
@@ -341,16 +341,10 @@
     <t>Property</t>
   </si>
   <si>
-    <t>32-24</t>
-  </si>
-  <si>
     <t>RESERVED</t>
   </si>
   <si>
     <t>RO</t>
-  </si>
-  <si>
-    <t>23-16</t>
   </si>
   <si>
     <t>BAUND</t>
@@ -375,9 +369,6 @@
     <t>UART busy.
 0 : UART is idle
 1 : UART is busy</t>
-  </si>
-  <si>
-    <t>14-1</t>
   </si>
   <si>
     <t>RegStructure</t>
@@ -445,6 +436,15 @@
   </si>
   <si>
     <t>No/Sync/Async</t>
+  </si>
+  <si>
+    <t>[32:28]</t>
+  </si>
+  <si>
+    <t>[27:24][23:16]</t>
+  </si>
+  <si>
+    <t>[14:8][7:1]</t>
   </si>
 </sst>
 </file>
@@ -969,28 +969,28 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1226,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -1267,10 +1267,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1278,12 +1278,12 @@
         <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>33</v>
@@ -1291,10 +1291,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -1302,12 +1302,12 @@
         <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B10" s="2">
         <v>32</v>
@@ -1343,30 +1343,30 @@
     </row>
     <row r="14" spans="1:4" ht="33" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="49.5" x14ac:dyDescent="0.35">
@@ -1374,27 +1374,27 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="33" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="49.5" x14ac:dyDescent="0.35">
@@ -1402,13 +1402,13 @@
         <v>0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update spec and lib
</commit_message>
<xml_diff>
--- a/input/RegSpec_Org.xlsx
+++ b/input/RegSpec_Org.xlsx
@@ -34,31 +34,7 @@
     <author>8560w</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>QuanNguyen:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Ver 1: Only support 32 bits</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0" shapeId="0">
+    <comment ref="B13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D14" authorId="0" shapeId="0">
+    <comment ref="D15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -152,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0">
+    <comment ref="D18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
   <si>
     <t>No</t>
   </si>
@@ -330,9 +306,6 @@
   </si>
   <si>
     <t>UART control register</t>
-  </si>
-  <si>
-    <t>Gen</t>
   </si>
   <si>
     <t>Bit</t>
@@ -371,9 +344,6 @@
 1 : UART is busy</t>
   </si>
   <si>
-    <t>RegStructure</t>
-  </si>
-  <si>
     <t>EN</t>
   </si>
   <si>
@@ -412,32 +382,6 @@
     <t>Write protection</t>
   </si>
   <si>
-    <t>Reserved/WProt/Sec</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>AXI4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>/APB4</t>
-    </r>
-  </si>
-  <si>
-    <t>No/Sync/Async</t>
-  </si>
-  <si>
     <t>Reset Value</t>
   </si>
   <si>
@@ -460,13 +404,40 @@
   </si>
   <si>
     <t>4'd0</t>
+  </si>
+  <si>
+    <t>Register specification of VG</t>
+  </si>
+  <si>
+    <t>APB4</t>
+  </si>
+  <si>
+    <t>No/Yes</t>
+  </si>
+  <si>
+    <t>WProt/Sec</t>
+  </si>
+  <si>
+    <t>DataWidth</t>
+  </si>
+  <si>
+    <t>AddrWidth</t>
+  </si>
+  <si>
+    <t>16'h0000</t>
+  </si>
+  <si>
+    <t>Gen/-</t>
+  </si>
+  <si>
+    <t>Only 32, not changed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="13"/>
       <color theme="1"/>
@@ -498,12 +469,6 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -987,28 +952,28 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1157,14 +1122,15 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.92578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1224,7 +1190,9 @@
       <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
@@ -1242,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -1277,7 +1245,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>32</v>
@@ -1285,10 +1253,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1296,155 +1264,169 @@
         <v>31</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>72</v>
+      </c>
+      <c r="B7" s="2">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
+      </c>
+      <c r="B8" s="2">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B13" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="B14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="4" t="s">
+      <c r="E14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="33" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="33" x14ac:dyDescent="0.35">
-      <c r="A14" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="49.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="49.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="33" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="49.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="5">
-        <v>0</v>
+    </row>
+    <row r="18" spans="1:5" ht="33" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>43</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>51</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="49.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5">
+        <v>0</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add scipts in work folder
</commit_message>
<xml_diff>
--- a/input/RegSpec_Org.xlsx
+++ b/input/RegSpec_Org.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\20.Project\3.Github\RegRTLGen\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\RegRTLGen\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="5" r:id="rId1"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="202">
   <si>
     <t>No</t>
   </si>
@@ -651,32 +651,6 @@
     <t>depend on 'Write_Protection' &amp; 'Secure'</t>
   </si>
   <si>
-    <r>
-      <t>RegSpec[RegSpec_Example]['Common_Config'][</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>'xxx'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>] = '...'</t>
-    </r>
-  </si>
-  <si>
-    <t>T.B.D</t>
-  </si>
-  <si>
     <t>RegSpec[RegSpec_Example][Register_No_1] = {}</t>
   </si>
   <si>
@@ -721,29 +695,6 @@
     <t>hex number</t>
   </si>
   <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config'][</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>'xxx'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>] = '…'</t>
-    </r>
-  </si>
-  <si>
     <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1] = {}</t>
   </si>
   <si>
@@ -770,36 +721,9 @@
     </r>
   </si>
   <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Field_Name'] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Field_Desciption'] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Strobe_No_1] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Strobe_No_1]['Bit_Range'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Strobe_No_1]['Reset_Value'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Strobe_No_1]['RW_Property'] = '…'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Strobe_No_1]['Pulse_Property'] = '…'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Strobe_No_2] = {}</t>
-  </si>
-  <si>
     <t>n</t>
   </si>
   <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Strobe_No_n] = {}</t>
-  </si>
-  <si>
     <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_2] = {}</t>
   </si>
   <si>
@@ -822,12 +746,177 @@
   </si>
   <si>
     <t>Yes/No</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>RW_Property</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = {}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Strobe_0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = []</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Strobe_1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = []</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Strobe_2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = []</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Strobe_3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = []</t>
+    </r>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_2] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_n] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['Bit_Range'] = '...'</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['Reset_Value'] = '...'</t>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Strobe_Index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = '…'</t>
+    </r>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['RW_Property'] = []</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config']['Field_Name'] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config']['Field_Desciption'] = {}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="13"/>
@@ -968,7 +1057,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1068,7 +1157,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1412,19 +1500,19 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -1432,7 +1520,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -1440,12 +1528,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>52</v>
       </c>
@@ -1464,17 +1552,17 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.78515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.35546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.77734375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1491,7 +1579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1508,7 +1596,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1543,15 +1631,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.35546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.2109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1562,7 +1650,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1573,7 +1661,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="66" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1584,7 +1672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1614,272 +1702,272 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.85546875" style="20" customWidth="1"/>
-    <col min="4" max="256" width="9.140625" style="20"/>
-    <col min="257" max="257" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="69.85546875" style="20" customWidth="1"/>
-    <col min="260" max="512" width="9.140625" style="20"/>
-    <col min="513" max="513" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="515" max="515" width="69.85546875" style="20" customWidth="1"/>
-    <col min="516" max="768" width="9.140625" style="20"/>
-    <col min="769" max="769" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="771" max="771" width="69.85546875" style="20" customWidth="1"/>
-    <col min="772" max="1024" width="9.140625" style="20"/>
-    <col min="1025" max="1025" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1027" max="1027" width="69.85546875" style="20" customWidth="1"/>
-    <col min="1028" max="1280" width="9.140625" style="20"/>
-    <col min="1281" max="1281" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1283" max="1283" width="69.85546875" style="20" customWidth="1"/>
-    <col min="1284" max="1536" width="9.140625" style="20"/>
-    <col min="1537" max="1537" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1539" max="1539" width="69.85546875" style="20" customWidth="1"/>
-    <col min="1540" max="1792" width="9.140625" style="20"/>
-    <col min="1793" max="1793" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1795" max="1795" width="69.85546875" style="20" customWidth="1"/>
-    <col min="1796" max="2048" width="9.140625" style="20"/>
-    <col min="2049" max="2049" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2051" max="2051" width="69.85546875" style="20" customWidth="1"/>
-    <col min="2052" max="2304" width="9.140625" style="20"/>
-    <col min="2305" max="2305" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2307" max="2307" width="69.85546875" style="20" customWidth="1"/>
-    <col min="2308" max="2560" width="9.140625" style="20"/>
-    <col min="2561" max="2561" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2563" max="2563" width="69.85546875" style="20" customWidth="1"/>
-    <col min="2564" max="2816" width="9.140625" style="20"/>
-    <col min="2817" max="2817" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2819" max="2819" width="69.85546875" style="20" customWidth="1"/>
-    <col min="2820" max="3072" width="9.140625" style="20"/>
-    <col min="3073" max="3073" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3075" max="3075" width="69.85546875" style="20" customWidth="1"/>
-    <col min="3076" max="3328" width="9.140625" style="20"/>
-    <col min="3329" max="3329" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3331" max="3331" width="69.85546875" style="20" customWidth="1"/>
-    <col min="3332" max="3584" width="9.140625" style="20"/>
-    <col min="3585" max="3585" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3587" max="3587" width="69.85546875" style="20" customWidth="1"/>
-    <col min="3588" max="3840" width="9.140625" style="20"/>
-    <col min="3841" max="3841" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3843" max="3843" width="69.85546875" style="20" customWidth="1"/>
-    <col min="3844" max="4096" width="9.140625" style="20"/>
-    <col min="4097" max="4097" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4099" max="4099" width="69.85546875" style="20" customWidth="1"/>
-    <col min="4100" max="4352" width="9.140625" style="20"/>
-    <col min="4353" max="4353" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4355" max="4355" width="69.85546875" style="20" customWidth="1"/>
-    <col min="4356" max="4608" width="9.140625" style="20"/>
-    <col min="4609" max="4609" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4611" max="4611" width="69.85546875" style="20" customWidth="1"/>
-    <col min="4612" max="4864" width="9.140625" style="20"/>
-    <col min="4865" max="4865" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4867" max="4867" width="69.85546875" style="20" customWidth="1"/>
-    <col min="4868" max="5120" width="9.140625" style="20"/>
-    <col min="5121" max="5121" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5123" max="5123" width="69.85546875" style="20" customWidth="1"/>
-    <col min="5124" max="5376" width="9.140625" style="20"/>
-    <col min="5377" max="5377" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5379" max="5379" width="69.85546875" style="20" customWidth="1"/>
-    <col min="5380" max="5632" width="9.140625" style="20"/>
-    <col min="5633" max="5633" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5635" max="5635" width="69.85546875" style="20" customWidth="1"/>
-    <col min="5636" max="5888" width="9.140625" style="20"/>
-    <col min="5889" max="5889" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5891" max="5891" width="69.85546875" style="20" customWidth="1"/>
-    <col min="5892" max="6144" width="9.140625" style="20"/>
-    <col min="6145" max="6145" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6147" max="6147" width="69.85546875" style="20" customWidth="1"/>
-    <col min="6148" max="6400" width="9.140625" style="20"/>
-    <col min="6401" max="6401" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6403" max="6403" width="69.85546875" style="20" customWidth="1"/>
-    <col min="6404" max="6656" width="9.140625" style="20"/>
-    <col min="6657" max="6657" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6659" max="6659" width="69.85546875" style="20" customWidth="1"/>
-    <col min="6660" max="6912" width="9.140625" style="20"/>
-    <col min="6913" max="6913" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6915" max="6915" width="69.85546875" style="20" customWidth="1"/>
-    <col min="6916" max="7168" width="9.140625" style="20"/>
-    <col min="7169" max="7169" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7171" max="7171" width="69.85546875" style="20" customWidth="1"/>
-    <col min="7172" max="7424" width="9.140625" style="20"/>
-    <col min="7425" max="7425" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7427" max="7427" width="69.85546875" style="20" customWidth="1"/>
-    <col min="7428" max="7680" width="9.140625" style="20"/>
-    <col min="7681" max="7681" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7683" max="7683" width="69.85546875" style="20" customWidth="1"/>
-    <col min="7684" max="7936" width="9.140625" style="20"/>
-    <col min="7937" max="7937" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7939" max="7939" width="69.85546875" style="20" customWidth="1"/>
-    <col min="7940" max="8192" width="9.140625" style="20"/>
-    <col min="8193" max="8193" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8195" max="8195" width="69.85546875" style="20" customWidth="1"/>
-    <col min="8196" max="8448" width="9.140625" style="20"/>
-    <col min="8449" max="8449" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8451" max="8451" width="69.85546875" style="20" customWidth="1"/>
-    <col min="8452" max="8704" width="9.140625" style="20"/>
-    <col min="8705" max="8705" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8707" max="8707" width="69.85546875" style="20" customWidth="1"/>
-    <col min="8708" max="8960" width="9.140625" style="20"/>
-    <col min="8961" max="8961" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8963" max="8963" width="69.85546875" style="20" customWidth="1"/>
-    <col min="8964" max="9216" width="9.140625" style="20"/>
-    <col min="9217" max="9217" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9219" max="9219" width="69.85546875" style="20" customWidth="1"/>
-    <col min="9220" max="9472" width="9.140625" style="20"/>
-    <col min="9473" max="9473" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9475" max="9475" width="69.85546875" style="20" customWidth="1"/>
-    <col min="9476" max="9728" width="9.140625" style="20"/>
-    <col min="9729" max="9729" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9731" max="9731" width="69.85546875" style="20" customWidth="1"/>
-    <col min="9732" max="9984" width="9.140625" style="20"/>
-    <col min="9985" max="9985" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9987" max="9987" width="69.85546875" style="20" customWidth="1"/>
-    <col min="9988" max="10240" width="9.140625" style="20"/>
-    <col min="10241" max="10241" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10243" max="10243" width="69.85546875" style="20" customWidth="1"/>
-    <col min="10244" max="10496" width="9.140625" style="20"/>
-    <col min="10497" max="10497" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10499" max="10499" width="69.85546875" style="20" customWidth="1"/>
-    <col min="10500" max="10752" width="9.140625" style="20"/>
-    <col min="10753" max="10753" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10755" max="10755" width="69.85546875" style="20" customWidth="1"/>
-    <col min="10756" max="11008" width="9.140625" style="20"/>
-    <col min="11009" max="11009" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11011" max="11011" width="69.85546875" style="20" customWidth="1"/>
-    <col min="11012" max="11264" width="9.140625" style="20"/>
-    <col min="11265" max="11265" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11267" max="11267" width="69.85546875" style="20" customWidth="1"/>
-    <col min="11268" max="11520" width="9.140625" style="20"/>
-    <col min="11521" max="11521" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11523" max="11523" width="69.85546875" style="20" customWidth="1"/>
-    <col min="11524" max="11776" width="9.140625" style="20"/>
-    <col min="11777" max="11777" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11779" max="11779" width="69.85546875" style="20" customWidth="1"/>
-    <col min="11780" max="12032" width="9.140625" style="20"/>
-    <col min="12033" max="12033" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12035" max="12035" width="69.85546875" style="20" customWidth="1"/>
-    <col min="12036" max="12288" width="9.140625" style="20"/>
-    <col min="12289" max="12289" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12291" max="12291" width="69.85546875" style="20" customWidth="1"/>
-    <col min="12292" max="12544" width="9.140625" style="20"/>
-    <col min="12545" max="12545" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12547" max="12547" width="69.85546875" style="20" customWidth="1"/>
-    <col min="12548" max="12800" width="9.140625" style="20"/>
-    <col min="12801" max="12801" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12803" max="12803" width="69.85546875" style="20" customWidth="1"/>
-    <col min="12804" max="13056" width="9.140625" style="20"/>
-    <col min="13057" max="13057" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13059" max="13059" width="69.85546875" style="20" customWidth="1"/>
-    <col min="13060" max="13312" width="9.140625" style="20"/>
-    <col min="13313" max="13313" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13315" max="13315" width="69.85546875" style="20" customWidth="1"/>
-    <col min="13316" max="13568" width="9.140625" style="20"/>
-    <col min="13569" max="13569" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13571" max="13571" width="69.85546875" style="20" customWidth="1"/>
-    <col min="13572" max="13824" width="9.140625" style="20"/>
-    <col min="13825" max="13825" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13827" max="13827" width="69.85546875" style="20" customWidth="1"/>
-    <col min="13828" max="14080" width="9.140625" style="20"/>
-    <col min="14081" max="14081" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14083" max="14083" width="69.85546875" style="20" customWidth="1"/>
-    <col min="14084" max="14336" width="9.140625" style="20"/>
-    <col min="14337" max="14337" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14339" max="14339" width="69.85546875" style="20" customWidth="1"/>
-    <col min="14340" max="14592" width="9.140625" style="20"/>
-    <col min="14593" max="14593" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14595" max="14595" width="69.85546875" style="20" customWidth="1"/>
-    <col min="14596" max="14848" width="9.140625" style="20"/>
-    <col min="14849" max="14849" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14851" max="14851" width="69.85546875" style="20" customWidth="1"/>
-    <col min="14852" max="15104" width="9.140625" style="20"/>
-    <col min="15105" max="15105" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15107" max="15107" width="69.85546875" style="20" customWidth="1"/>
-    <col min="15108" max="15360" width="9.140625" style="20"/>
-    <col min="15361" max="15361" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15363" max="15363" width="69.85546875" style="20" customWidth="1"/>
-    <col min="15364" max="15616" width="9.140625" style="20"/>
-    <col min="15617" max="15617" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15619" max="15619" width="69.85546875" style="20" customWidth="1"/>
-    <col min="15620" max="15872" width="9.140625" style="20"/>
-    <col min="15873" max="15873" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15875" max="15875" width="69.85546875" style="20" customWidth="1"/>
-    <col min="15876" max="16128" width="9.140625" style="20"/>
-    <col min="16129" max="16129" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
-    <col min="16131" max="16131" width="69.85546875" style="20" customWidth="1"/>
-    <col min="16132" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="4.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.88671875" style="20" customWidth="1"/>
+    <col min="4" max="256" width="9.109375" style="20"/>
+    <col min="257" max="257" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="69.88671875" style="20" customWidth="1"/>
+    <col min="260" max="512" width="9.109375" style="20"/>
+    <col min="513" max="513" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="69.88671875" style="20" customWidth="1"/>
+    <col min="516" max="768" width="9.109375" style="20"/>
+    <col min="769" max="769" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="771" max="771" width="69.88671875" style="20" customWidth="1"/>
+    <col min="772" max="1024" width="9.109375" style="20"/>
+    <col min="1025" max="1025" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1027" width="69.88671875" style="20" customWidth="1"/>
+    <col min="1028" max="1280" width="9.109375" style="20"/>
+    <col min="1281" max="1281" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1283" width="69.88671875" style="20" customWidth="1"/>
+    <col min="1284" max="1536" width="9.109375" style="20"/>
+    <col min="1537" max="1537" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1539" width="69.88671875" style="20" customWidth="1"/>
+    <col min="1540" max="1792" width="9.109375" style="20"/>
+    <col min="1793" max="1793" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1795" width="69.88671875" style="20" customWidth="1"/>
+    <col min="1796" max="2048" width="9.109375" style="20"/>
+    <col min="2049" max="2049" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2051" width="69.88671875" style="20" customWidth="1"/>
+    <col min="2052" max="2304" width="9.109375" style="20"/>
+    <col min="2305" max="2305" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2307" width="69.88671875" style="20" customWidth="1"/>
+    <col min="2308" max="2560" width="9.109375" style="20"/>
+    <col min="2561" max="2561" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2563" width="69.88671875" style="20" customWidth="1"/>
+    <col min="2564" max="2816" width="9.109375" style="20"/>
+    <col min="2817" max="2817" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2819" width="69.88671875" style="20" customWidth="1"/>
+    <col min="2820" max="3072" width="9.109375" style="20"/>
+    <col min="3073" max="3073" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3075" width="69.88671875" style="20" customWidth="1"/>
+    <col min="3076" max="3328" width="9.109375" style="20"/>
+    <col min="3329" max="3329" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3331" width="69.88671875" style="20" customWidth="1"/>
+    <col min="3332" max="3584" width="9.109375" style="20"/>
+    <col min="3585" max="3585" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3587" width="69.88671875" style="20" customWidth="1"/>
+    <col min="3588" max="3840" width="9.109375" style="20"/>
+    <col min="3841" max="3841" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3843" width="69.88671875" style="20" customWidth="1"/>
+    <col min="3844" max="4096" width="9.109375" style="20"/>
+    <col min="4097" max="4097" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4099" width="69.88671875" style="20" customWidth="1"/>
+    <col min="4100" max="4352" width="9.109375" style="20"/>
+    <col min="4353" max="4353" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4355" width="69.88671875" style="20" customWidth="1"/>
+    <col min="4356" max="4608" width="9.109375" style="20"/>
+    <col min="4609" max="4609" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4611" width="69.88671875" style="20" customWidth="1"/>
+    <col min="4612" max="4864" width="9.109375" style="20"/>
+    <col min="4865" max="4865" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4867" width="69.88671875" style="20" customWidth="1"/>
+    <col min="4868" max="5120" width="9.109375" style="20"/>
+    <col min="5121" max="5121" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5123" width="69.88671875" style="20" customWidth="1"/>
+    <col min="5124" max="5376" width="9.109375" style="20"/>
+    <col min="5377" max="5377" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5379" width="69.88671875" style="20" customWidth="1"/>
+    <col min="5380" max="5632" width="9.109375" style="20"/>
+    <col min="5633" max="5633" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5635" width="69.88671875" style="20" customWidth="1"/>
+    <col min="5636" max="5888" width="9.109375" style="20"/>
+    <col min="5889" max="5889" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5891" width="69.88671875" style="20" customWidth="1"/>
+    <col min="5892" max="6144" width="9.109375" style="20"/>
+    <col min="6145" max="6145" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6147" width="69.88671875" style="20" customWidth="1"/>
+    <col min="6148" max="6400" width="9.109375" style="20"/>
+    <col min="6401" max="6401" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6403" width="69.88671875" style="20" customWidth="1"/>
+    <col min="6404" max="6656" width="9.109375" style="20"/>
+    <col min="6657" max="6657" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6659" width="69.88671875" style="20" customWidth="1"/>
+    <col min="6660" max="6912" width="9.109375" style="20"/>
+    <col min="6913" max="6913" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6915" width="69.88671875" style="20" customWidth="1"/>
+    <col min="6916" max="7168" width="9.109375" style="20"/>
+    <col min="7169" max="7169" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7171" width="69.88671875" style="20" customWidth="1"/>
+    <col min="7172" max="7424" width="9.109375" style="20"/>
+    <col min="7425" max="7425" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7427" width="69.88671875" style="20" customWidth="1"/>
+    <col min="7428" max="7680" width="9.109375" style="20"/>
+    <col min="7681" max="7681" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7683" width="69.88671875" style="20" customWidth="1"/>
+    <col min="7684" max="7936" width="9.109375" style="20"/>
+    <col min="7937" max="7937" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7939" width="69.88671875" style="20" customWidth="1"/>
+    <col min="7940" max="8192" width="9.109375" style="20"/>
+    <col min="8193" max="8193" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8195" width="69.88671875" style="20" customWidth="1"/>
+    <col min="8196" max="8448" width="9.109375" style="20"/>
+    <col min="8449" max="8449" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8451" width="69.88671875" style="20" customWidth="1"/>
+    <col min="8452" max="8704" width="9.109375" style="20"/>
+    <col min="8705" max="8705" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8707" width="69.88671875" style="20" customWidth="1"/>
+    <col min="8708" max="8960" width="9.109375" style="20"/>
+    <col min="8961" max="8961" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8963" width="69.88671875" style="20" customWidth="1"/>
+    <col min="8964" max="9216" width="9.109375" style="20"/>
+    <col min="9217" max="9217" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9219" width="69.88671875" style="20" customWidth="1"/>
+    <col min="9220" max="9472" width="9.109375" style="20"/>
+    <col min="9473" max="9473" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9475" width="69.88671875" style="20" customWidth="1"/>
+    <col min="9476" max="9728" width="9.109375" style="20"/>
+    <col min="9729" max="9729" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9731" width="69.88671875" style="20" customWidth="1"/>
+    <col min="9732" max="9984" width="9.109375" style="20"/>
+    <col min="9985" max="9985" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9987" width="69.88671875" style="20" customWidth="1"/>
+    <col min="9988" max="10240" width="9.109375" style="20"/>
+    <col min="10241" max="10241" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10243" width="69.88671875" style="20" customWidth="1"/>
+    <col min="10244" max="10496" width="9.109375" style="20"/>
+    <col min="10497" max="10497" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10499" width="69.88671875" style="20" customWidth="1"/>
+    <col min="10500" max="10752" width="9.109375" style="20"/>
+    <col min="10753" max="10753" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10755" width="69.88671875" style="20" customWidth="1"/>
+    <col min="10756" max="11008" width="9.109375" style="20"/>
+    <col min="11009" max="11009" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11011" width="69.88671875" style="20" customWidth="1"/>
+    <col min="11012" max="11264" width="9.109375" style="20"/>
+    <col min="11265" max="11265" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11267" width="69.88671875" style="20" customWidth="1"/>
+    <col min="11268" max="11520" width="9.109375" style="20"/>
+    <col min="11521" max="11521" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11523" width="69.88671875" style="20" customWidth="1"/>
+    <col min="11524" max="11776" width="9.109375" style="20"/>
+    <col min="11777" max="11777" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11779" width="69.88671875" style="20" customWidth="1"/>
+    <col min="11780" max="12032" width="9.109375" style="20"/>
+    <col min="12033" max="12033" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12035" width="69.88671875" style="20" customWidth="1"/>
+    <col min="12036" max="12288" width="9.109375" style="20"/>
+    <col min="12289" max="12289" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12291" width="69.88671875" style="20" customWidth="1"/>
+    <col min="12292" max="12544" width="9.109375" style="20"/>
+    <col min="12545" max="12545" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12547" width="69.88671875" style="20" customWidth="1"/>
+    <col min="12548" max="12800" width="9.109375" style="20"/>
+    <col min="12801" max="12801" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12803" width="69.88671875" style="20" customWidth="1"/>
+    <col min="12804" max="13056" width="9.109375" style="20"/>
+    <col min="13057" max="13057" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13059" width="69.88671875" style="20" customWidth="1"/>
+    <col min="13060" max="13312" width="9.109375" style="20"/>
+    <col min="13313" max="13313" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13315" width="69.88671875" style="20" customWidth="1"/>
+    <col min="13316" max="13568" width="9.109375" style="20"/>
+    <col min="13569" max="13569" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13571" width="69.88671875" style="20" customWidth="1"/>
+    <col min="13572" max="13824" width="9.109375" style="20"/>
+    <col min="13825" max="13825" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13827" width="69.88671875" style="20" customWidth="1"/>
+    <col min="13828" max="14080" width="9.109375" style="20"/>
+    <col min="14081" max="14081" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14083" width="69.88671875" style="20" customWidth="1"/>
+    <col min="14084" max="14336" width="9.109375" style="20"/>
+    <col min="14337" max="14337" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14339" width="69.88671875" style="20" customWidth="1"/>
+    <col min="14340" max="14592" width="9.109375" style="20"/>
+    <col min="14593" max="14593" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14595" width="69.88671875" style="20" customWidth="1"/>
+    <col min="14596" max="14848" width="9.109375" style="20"/>
+    <col min="14849" max="14849" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14851" width="69.88671875" style="20" customWidth="1"/>
+    <col min="14852" max="15104" width="9.109375" style="20"/>
+    <col min="15105" max="15105" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15107" width="69.88671875" style="20" customWidth="1"/>
+    <col min="15108" max="15360" width="9.109375" style="20"/>
+    <col min="15361" max="15361" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15363" width="69.88671875" style="20" customWidth="1"/>
+    <col min="15364" max="15616" width="9.109375" style="20"/>
+    <col min="15617" max="15617" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15619" width="69.88671875" style="20" customWidth="1"/>
+    <col min="15620" max="15872" width="9.109375" style="20"/>
+    <col min="15873" max="15873" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15875" width="69.88671875" style="20" customWidth="1"/>
+    <col min="15876" max="16128" width="9.109375" style="20"/>
+    <col min="16129" max="16129" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16131" width="69.88671875" style="20" customWidth="1"/>
+    <col min="16132" max="16384" width="9.109375" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>77</v>
       </c>
@@ -1890,7 +1978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -1901,7 +1989,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A4" s="21">
         <v>2</v>
       </c>
@@ -1912,7 +2000,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A5" s="21">
         <v>3</v>
       </c>
@@ -1923,7 +2011,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
         <v>4</v>
       </c>
@@ -1934,7 +2022,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>5</v>
       </c>
@@ -1945,7 +2033,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
         <v>6</v>
       </c>
@@ -1956,7 +2044,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
         <v>7</v>
       </c>
@@ -1967,7 +2055,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
         <v>8</v>
       </c>
@@ -1978,7 +2066,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
         <v>9</v>
       </c>
@@ -1989,7 +2077,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
         <v>10</v>
       </c>
@@ -2000,7 +2088,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
         <v>11</v>
       </c>
@@ -2011,7 +2099,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
         <v>12</v>
       </c>
@@ -2022,7 +2110,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
         <v>13</v>
       </c>
@@ -2033,7 +2121,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
         <v>14</v>
       </c>
@@ -2044,7 +2132,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
         <v>15</v>
       </c>
@@ -2055,7 +2143,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
         <v>16</v>
       </c>
@@ -2066,7 +2154,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="21">
         <v>17</v>
       </c>
@@ -2077,7 +2165,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
         <v>18</v>
       </c>
@@ -2088,12 +2176,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="27" t="s">
         <v>77</v>
       </c>
@@ -2104,7 +2192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A24" s="21">
         <v>1</v>
       </c>
@@ -2115,7 +2203,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A25" s="21">
         <v>2</v>
       </c>
@@ -2126,7 +2214,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A26" s="21">
         <v>3</v>
       </c>
@@ -2137,7 +2225,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="40" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
       <c r="A27" s="21">
         <v>4</v>
       </c>
@@ -2162,25 +2250,25 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="11"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2191,7 +2279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -2202,7 +2290,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -2213,7 +2301,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>21</v>
@@ -2222,7 +2310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
@@ -2231,7 +2319,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2249,27 +2337,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.2109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.78515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.35546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
@@ -2280,7 +2368,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -2288,15 +2376,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
@@ -2304,7 +2392,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -2312,7 +2400,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>69</v>
       </c>
@@ -2323,7 +2411,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>70</v>
       </c>
@@ -2331,7 +2419,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>147</v>
       </c>
@@ -2339,7 +2427,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
@@ -2347,7 +2435,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>136</v>
       </c>
@@ -2358,7 +2446,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
@@ -2366,7 +2454,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>135</v>
       </c>
@@ -2374,7 +2462,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
@@ -2385,7 +2473,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>27</v>
       </c>
@@ -2402,7 +2490,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -2419,7 +2507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>63</v>
       </c>
@@ -2436,7 +2524,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>59</v>
       </c>
@@ -2453,7 +2541,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>15</v>
       </c>
@@ -2470,7 +2558,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>58</v>
       </c>
@@ -2487,7 +2575,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="49.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>0</v>
       </c>
@@ -2504,7 +2592,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>27</v>
       </c>
@@ -2521,7 +2609,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
@@ -2538,7 +2626,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>63</v>
       </c>
@@ -2553,7 +2641,7 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>59</v>
       </c>
@@ -2568,7 +2656,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>128</v>
       </c>
@@ -2583,7 +2671,7 @@
       </c>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
         <v>126</v>
       </c>
@@ -2598,7 +2686,7 @@
       </c>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>0</v>
       </c>
@@ -2630,12 +2718,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>139</v>
       </c>
@@ -2646,7 +2734,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>141</v>
       </c>
@@ -2657,7 +2745,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>1</v>
       </c>
@@ -2665,7 +2753,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>2</v>
       </c>
@@ -2673,7 +2761,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>3</v>
       </c>
@@ -2681,7 +2769,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>148</v>
       </c>
@@ -2692,12 +2780,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="30" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>150</v>
       </c>
@@ -2709,20 +2797,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:T44"/>
+  <dimension ref="B3:T48"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R42" sqref="R42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="31">
         <v>0</v>
       </c>
@@ -2733,7 +2821,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="32">
         <v>1</v>
       </c>
@@ -2741,7 +2829,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="33"/>
       <c r="C6" s="31">
         <v>0</v>
@@ -2750,7 +2838,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
       <c r="E7" t="s">
@@ -2760,7 +2848,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="33"/>
       <c r="C8" s="33"/>
       <c r="E8" t="s">
@@ -2770,7 +2858,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="33"/>
       <c r="C9" s="33"/>
       <c r="E9" t="s">
@@ -2780,7 +2868,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="33"/>
       <c r="C10" s="33"/>
       <c r="E10" t="s">
@@ -2790,7 +2878,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="33"/>
       <c r="C11" s="33"/>
       <c r="E11" t="s">
@@ -2800,7 +2888,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="33"/>
       <c r="C12" s="33"/>
       <c r="E12" t="s">
@@ -2810,7 +2898,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="33"/>
       <c r="C13" s="33"/>
       <c r="E13" t="s">
@@ -2820,7 +2908,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="33"/>
       <c r="C14" s="33"/>
       <c r="E14" t="s">
@@ -2830,7 +2918,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="33"/>
       <c r="C15" s="33"/>
       <c r="E15" t="s">
@@ -2840,7 +2928,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
       <c r="E16" t="s">
@@ -2850,40 +2938,41 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B17" s="33"/>
       <c r="C17" s="33"/>
-      <c r="E17" t="s">
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B18" s="33"/>
+      <c r="C18" s="32">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
         <v>168</v>
       </c>
-      <c r="M17" s="35" t="s">
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="31">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B19" s="33"/>
-      <c r="C19" s="32">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="33"/>
       <c r="C20" s="33"/>
-      <c r="D20" s="31">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D20" s="33"/>
+      <c r="F20" t="s">
+        <v>170</v>
+      </c>
+      <c r="P20" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="33"/>
       <c r="C21" s="33"/>
       <c r="D21" s="33"/>
@@ -2891,242 +2980,279 @@
         <v>172</v>
       </c>
       <c r="P21" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
       <c r="D22" s="33"/>
       <c r="F22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P22" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
       <c r="D23" s="33"/>
       <c r="F23" t="s">
+        <v>174</v>
+      </c>
+      <c r="P23" t="s">
         <v>175</v>
       </c>
-      <c r="P23" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="33"/>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
       <c r="F24" t="s">
-        <v>176</v>
-      </c>
-      <c r="P24" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.35">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="33"/>
       <c r="C25" s="33"/>
       <c r="D25" s="33"/>
       <c r="F25" t="s">
-        <v>178</v>
-      </c>
-      <c r="P25" s="35" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="P25" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="33"/>
       <c r="C26" s="33"/>
       <c r="D26" s="33"/>
-    </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>190</v>
+      </c>
+      <c r="P26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="33"/>
       <c r="C27" s="33"/>
-      <c r="D27" s="32">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="D27" s="33"/>
+      <c r="F27" t="s">
+        <v>191</v>
+      </c>
+      <c r="P27" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B28" s="33"/>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
-      <c r="E28" s="31">
-        <v>0</v>
-      </c>
       <c r="F28" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+      <c r="P28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="33"/>
       <c r="C29" s="33"/>
       <c r="D29" s="33"/>
-      <c r="E29" s="33"/>
-      <c r="G29" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="33"/>
       <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="G30" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="D30" s="32">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="33"/>
       <c r="C31" s="33"/>
       <c r="D31" s="33"/>
-      <c r="E31" s="32">
-        <v>1</v>
+      <c r="E31" s="31">
+        <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="33"/>
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
       <c r="G32" t="s">
-        <v>184</v>
-      </c>
-      <c r="T32" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="33"/>
       <c r="C33" s="33"/>
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="G33" t="s">
-        <v>185</v>
-      </c>
-      <c r="T33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
-      <c r="G34" t="s">
-        <v>186</v>
-      </c>
-      <c r="T34" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B35" s="33"/>
       <c r="C35" s="33"/>
       <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="G35" t="s">
-        <v>187</v>
-      </c>
-      <c r="T35" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="E35" s="32">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B36" s="33"/>
       <c r="C36" s="33"/>
       <c r="D36" s="33"/>
-      <c r="E36" s="32">
-        <v>2</v>
-      </c>
-      <c r="F36" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="E36" s="33"/>
+      <c r="G36" t="s">
+        <v>196</v>
+      </c>
+      <c r="T36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B37" s="33"/>
       <c r="C37" s="33"/>
       <c r="D37" s="33"/>
-      <c r="E37" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="F37" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="E37" s="33"/>
+      <c r="G37" t="s">
+        <v>197</v>
+      </c>
+      <c r="T37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B38" s="33"/>
       <c r="C38" s="33"/>
-      <c r="D38" s="32">
-        <v>2</v>
-      </c>
-      <c r="E38" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="G38" t="s">
+        <v>198</v>
+      </c>
+      <c r="T38" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B39" s="33"/>
       <c r="C39" s="33"/>
-      <c r="D39" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="E39" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="G39" t="s">
+        <v>199</v>
+      </c>
+      <c r="T39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B40" s="33"/>
-      <c r="C40" s="32">
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="32">
         <v>2</v>
       </c>
-      <c r="D40" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="F40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B41" s="33"/>
-      <c r="C41" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="D41" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B42" s="32">
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="F41" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
+      <c r="D42" s="32">
         <v>2</v>
       </c>
-      <c r="C42" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B43" s="32" t="s">
-        <v>189</v>
-      </c>
-      <c r="C43" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.35">
+      <c r="E42" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B44" s="33"/>
+      <c r="C44" s="32">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="33"/>
+      <c r="C45" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="D45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B46" s="32">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B47" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C47" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B48" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
gen rtl - trial version
</commit_message>
<xml_diff>
--- a/input/RegSpec_Org.xlsx
+++ b/input/RegSpec_Org.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="5" r:id="rId1"/>
@@ -17,9 +17,10 @@
     <sheet name="Summary" sheetId="4" r:id="rId3"/>
     <sheet name="RegProperty" sheetId="6" r:id="rId4"/>
     <sheet name="CommonInfo" sheetId="2" r:id="rId5"/>
-    <sheet name="RegSpec_Example" sheetId="3" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
-    <sheet name="Variable_Structure" sheetId="8" r:id="rId8"/>
+    <sheet name="RegSpec_Test" sheetId="9" r:id="rId6"/>
+    <sheet name="RegSpec_Example" sheetId="3" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId8"/>
+    <sheet name="Variable_Structure" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -88,8 +89,66 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>8560w</author>
+  </authors>
+  <commentList>
+    <comment ref="B10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>8560w:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+$GenAsyncReset</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>8560w:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+$GenRegName</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="209">
   <si>
     <t>No</t>
   </si>
@@ -561,6 +620,87 @@
   </si>
   <si>
     <t>RegSpec = {}</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example]['Common_Config']['Interface'] = '...'</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1] = {}</t>
+  </si>
+  <si>
+    <t>0/1</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Register_Description'] = '…'</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Initial_Value'] = '…'</t>
+  </si>
+  <si>
+    <t>hex number</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1] = {}</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_2] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_n] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_2] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_n] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example_2] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example_n] = {}</t>
+  </si>
+  <si>
+    <t>Gen</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_2] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_n] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['RW_Property'] = []</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Async</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <r>
@@ -573,7 +713,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>'Common_Info'</t>
+      <t>'GenUserHeader'</t>
     </r>
     <r>
       <rPr>
@@ -586,14 +726,47 @@
     </r>
   </si>
   <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example] = {}</t>
-  </si>
-  <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][</t>
+    <t>RegSpec[RegSpec_Example]['Common_Config'] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config'] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property'] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['Strobe_0'] = []</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['Strobe_1'] = []</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['Strobe_2'] = []</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['Strobe_3'] = []</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config'] = {}</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config']['Field_Desciption'] = '…'</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config']['RW_Property'] = []</t>
+  </si>
+  <si>
+    <t>$GenStartLoop$GenRegName</t>
+  </si>
+  <si>
+    <t>$GenStartLoop$GenRegName$GenRegField</t>
+  </si>
+  <si>
+    <t>$GenStartLoop$GenRegName$GenRegField$GenPartialBitRange</t>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
     </r>
     <r>
       <rPr>
@@ -602,7 +775,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>'Common_Config'</t>
+      <t>GenModuleName</t>
     </r>
     <r>
       <rPr>
@@ -611,51 +784,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>] = {}</t>
-    </r>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['Module_Name'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['Interface'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['DataWidth'] = 32</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['AddrWidth'] = '...'</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['Reset'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['Synchronization'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['SynchronousStage'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['Write_Protection'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['Secure'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example]['Common_Config']['SlaveError'] = '...'</t>
-  </si>
-  <si>
-    <t>depend on 'Write_Protection' &amp; 'Secure'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1] = {}</t>
-  </si>
-  <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][Register_No_1][</t>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
     </r>
     <r>
       <rPr>
@@ -664,7 +798,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>'Common_Config'</t>
+      <t>GenDataParam</t>
     </r>
     <r>
       <rPr>
@@ -673,33 +807,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>] = {}</t>
-    </r>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Generate_Flag'] = '…'</t>
-  </si>
-  <si>
-    <t>0/1</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Register_Name'] = '…'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Register_Description'] = '…'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Initial_Value'] = '…'</t>
-  </si>
-  <si>
-    <t>hex number</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1] = {}</t>
-  </si>
-  <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][</t>
+      <t>'] = 32</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
     </r>
     <r>
       <rPr>
@@ -708,7 +821,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>'Common_Config'</t>
+      <t>GenAddrParam</t>
     </r>
     <r>
       <rPr>
@@ -717,51 +830,21 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>] = {}</t>
-    </r>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_2] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_n] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_2] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_n] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example_2] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example_n] = {}</t>
-  </si>
-  <si>
-    <t>Gen</t>
-  </si>
-  <si>
-    <t>Yes/No</t>
-  </si>
-  <si>
-    <t>list</t>
-  </si>
-  <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['</t>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
     </r>
     <r>
       <rPr>
         <sz val="13"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>RW_Property</t>
+      <t>GenSyncReset</t>
     </r>
     <r>
       <rPr>
@@ -770,21 +853,21 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>'] = {}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['</t>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
     </r>
     <r>
       <rPr>
         <sz val="13"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Strobe_0</t>
+      <t>GenAsyncReset</t>
     </r>
     <r>
       <rPr>
@@ -793,21 +876,21 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>'] = []</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['</t>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
     </r>
     <r>
       <rPr>
         <sz val="13"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Strobe_1</t>
+      <t>GenAsyncParam</t>
     </r>
     <r>
       <rPr>
@@ -816,21 +899,21 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>'] = []</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['</t>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
     </r>
     <r>
       <rPr>
         <sz val="13"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Strobe_2</t>
+      <t>GenSyncStageParam</t>
     </r>
     <r>
       <rPr>
@@ -839,21 +922,21 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>'] = []</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['RW_Property']['</t>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
     </r>
     <r>
       <rPr>
         <sz val="13"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Strobe_3</t>
+      <t>GenWProtParam</t>
     </r>
     <r>
       <rPr>
@@ -862,36 +945,90 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>'] = []</t>
-    </r>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_2] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_n] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['Bit_Range'] = '...'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['Reset_Value'] = '...'</t>
-  </si>
-  <si>
-    <r>
-      <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['</t>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
     </r>
     <r>
       <rPr>
         <sz val="13"/>
-        <color rgb="FFFF0000"/>
+        <color rgb="FF0070C0"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Strobe_Index</t>
+      <t>GenSecParam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GenWProtErrParam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example]['Common_Config']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GenSecErrParam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GenRegName</t>
     </r>
     <r>
       <rPr>
@@ -904,20 +1041,102 @@
     </r>
   </si>
   <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['RW_Property'] = []</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config']['Field_Name'] = {}</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config']['Field_Desciption'] = {}</t>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GenRegField</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = '…'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GenPartialBitRange</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GenFieldReset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = '...'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1][Register_Field_Split_No_1]['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GenPStrbIndex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = '...'</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="13"/>
       <color theme="1"/>
@@ -973,6 +1192,11 @@
     <font>
       <sz val="13"/>
       <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1057,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1157,6 +1381,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1226,6 +1451,152 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2585357" y="3973286"/>
+          <a:ext cx="1129393" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>503464</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>108857</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3551464" y="6218465"/>
+          <a:ext cx="1129393" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>530678</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>231321</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>108857</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5102678" y="7443108"/>
+          <a:ext cx="462643" cy="13606"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2338,7 +2709,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2378,10 +2749,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2424,7 +2795,7 @@
         <v>147</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2432,7 +2803,7 @@
         <v>55</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2440,7 +2811,7 @@
         <v>136</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>138</v>
@@ -2451,7 +2822,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>67</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2459,7 +2830,7 @@
         <v>135</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>67</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2478,7 +2849,7 @@
         <v>27</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>72</v>
+        <v>169</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>74</v>
@@ -2711,6 +3082,383 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="2">
+        <v>32</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>15</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>0</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>0</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Summary!A1" display="Back to summary"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D9"/>
   <sheetViews>
@@ -2795,464 +3543,556 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:T48"/>
+  <dimension ref="A3:W50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R42" sqref="R42"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="3" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="31">
+    <row r="4" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E4" s="31">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>179</v>
+      </c>
+      <c r="N4" t="s">
         <v>152</v>
       </c>
-      <c r="K4" t="s">
+    </row>
+    <row r="5" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E5" s="32">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="32">
+    <row r="6" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E6" s="33"/>
+      <c r="F6" s="31">
+        <v>0</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+      <c r="H7" t="s">
+        <v>193</v>
+      </c>
+      <c r="P7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="H8" t="s">
+        <v>154</v>
+      </c>
+      <c r="P8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="H9" t="s">
+        <v>194</v>
+      </c>
+      <c r="P9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="H10" t="s">
+        <v>195</v>
+      </c>
+      <c r="P10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="H11" t="s">
+        <v>196</v>
+      </c>
+      <c r="P11" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="H12" t="s">
+        <v>197</v>
+      </c>
+      <c r="P12" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="H13" t="s">
+        <v>198</v>
+      </c>
+      <c r="P13" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="H14" t="s">
+        <v>199</v>
+      </c>
+      <c r="P14" s="34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="H15" t="s">
+        <v>200</v>
+      </c>
+      <c r="P15" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="5:16" x14ac:dyDescent="0.25">
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="H16" t="s">
+        <v>201</v>
+      </c>
+      <c r="P16" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="H17" t="s">
+        <v>202</v>
+      </c>
+      <c r="P17" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="H18" t="s">
+        <v>203</v>
+      </c>
+      <c r="P18" s="30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="33"/>
+      <c r="F20" s="32">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="33"/>
-      <c r="C6" s="31">
+      <c r="G20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="31">
         <v>0</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H21" s="35" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+      <c r="I22" t="s">
+        <v>204</v>
+      </c>
+      <c r="S22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="33"/>
+      <c r="I23" t="s">
+        <v>158</v>
+      </c>
+      <c r="S23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="I24" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="T24" s="35"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="I25" s="35" t="s">
+        <v>182</v>
+      </c>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="35"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="I26" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="35"/>
+      <c r="R26" s="35"/>
+      <c r="S26" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="T26" s="35"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="I27" s="35" t="s">
+        <v>184</v>
+      </c>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="T27" s="35"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="I28" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
+      <c r="P28" s="35"/>
+      <c r="Q28" s="35"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="T28" s="35"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="I29" s="35" t="s">
+        <v>186</v>
+      </c>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+      <c r="N29" s="35"/>
+      <c r="O29" s="35"/>
+      <c r="P29" s="35"/>
+      <c r="Q29" s="35"/>
+      <c r="R29" s="35"/>
+      <c r="S29" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="T29" s="35"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>191</v>
+      </c>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="32">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="31">
+        <v>0</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="J33" t="s">
+        <v>205</v>
+      </c>
+      <c r="V33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E34" s="33"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="J34" t="s">
+        <v>188</v>
+      </c>
+      <c r="V34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="J35" t="s">
+        <v>189</v>
+      </c>
+      <c r="V35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>192</v>
+      </c>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="32">
+        <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="J38" t="s">
+        <v>206</v>
+      </c>
+      <c r="W38" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="E7" t="s">
-        <v>156</v>
-      </c>
-      <c r="M7" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="E8" t="s">
-        <v>157</v>
-      </c>
-      <c r="M8" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="E9" t="s">
-        <v>158</v>
-      </c>
-      <c r="M9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="E10" t="s">
-        <v>159</v>
-      </c>
-      <c r="M10" t="s">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="J39" t="s">
+        <v>207</v>
+      </c>
+      <c r="W39" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="E11" t="s">
-        <v>161</v>
-      </c>
-      <c r="M11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="E12" t="s">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="J40" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="W40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="J41" t="s">
+        <v>175</v>
+      </c>
+      <c r="W41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="32">
+        <v>2</v>
+      </c>
+      <c r="I42" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="M12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="E13" t="s">
+      <c r="I43" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E44" s="33"/>
+      <c r="F44" s="33"/>
+      <c r="G44" s="32">
+        <v>2</v>
+      </c>
+      <c r="H44" t="s">
         <v>163</v>
       </c>
-      <c r="M13" s="34" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="E14" t="s">
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E45" s="33"/>
+      <c r="F45" s="33"/>
+      <c r="G45" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="H45" t="s">
         <v>164</v>
       </c>
-      <c r="M14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="E15" t="s">
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E46" s="33"/>
+      <c r="F46" s="32">
+        <v>2</v>
+      </c>
+      <c r="G46" t="s">
         <v>165</v>
       </c>
-      <c r="M15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="E16" t="s">
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E47" s="33"/>
+      <c r="F47" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="G47" t="s">
         <v>166</v>
       </c>
-      <c r="M16" t="s">
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E48" s="32">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="33"/>
-      <c r="C18" s="32">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="49" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E49" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="F49" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="31">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="33"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="F20" t="s">
-        <v>170</v>
-      </c>
-      <c r="P20" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="F21" t="s">
-        <v>172</v>
-      </c>
-      <c r="P21" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="F22" t="s">
-        <v>173</v>
-      </c>
-      <c r="P22" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B23" s="33"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="F23" t="s">
-        <v>174</v>
-      </c>
-      <c r="P23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="F24" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-      <c r="F25" t="s">
-        <v>189</v>
-      </c>
-      <c r="P25" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="F26" t="s">
-        <v>190</v>
-      </c>
-      <c r="P26" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="F27" t="s">
-        <v>191</v>
-      </c>
-      <c r="P27" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="F28" t="s">
-        <v>192</v>
-      </c>
-      <c r="P28" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="32">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="31">
-        <v>0</v>
-      </c>
-      <c r="F31" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B32" s="33"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="G32" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="G33" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B34" s="33"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-    </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="32">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B36" s="33"/>
-      <c r="C36" s="33"/>
-      <c r="D36" s="33"/>
-      <c r="E36" s="33"/>
-      <c r="G36" t="s">
-        <v>196</v>
-      </c>
-      <c r="T36" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="G37" t="s">
-        <v>197</v>
-      </c>
-      <c r="T37" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B38" s="33"/>
-      <c r="C38" s="33"/>
-      <c r="D38" s="33"/>
-      <c r="E38" s="33"/>
-      <c r="G38" t="s">
-        <v>198</v>
-      </c>
-      <c r="T38" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="33"/>
-      <c r="E39" s="33"/>
-      <c r="G39" t="s">
-        <v>199</v>
-      </c>
-      <c r="T39" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B40" s="33"/>
-      <c r="C40" s="33"/>
-      <c r="D40" s="33"/>
-      <c r="E40" s="32">
-        <v>2</v>
-      </c>
-      <c r="F40" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="F41" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B42" s="33"/>
-      <c r="C42" s="33"/>
-      <c r="D42" s="32">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="E43" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B44" s="33"/>
-      <c r="C44" s="32">
-        <v>2</v>
-      </c>
-      <c r="D44" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B45" s="33"/>
-      <c r="C45" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="D45" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B46" s="32">
-        <v>2</v>
-      </c>
-      <c r="C46" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B47" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="C47" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B48" s="33"/>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E50" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete gen RTL, HTML
</commit_message>
<xml_diff>
--- a/input/RegSpec_Org.xlsx
+++ b/input/RegSpec_Org.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="5" r:id="rId1"/>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="241">
   <si>
     <t>No</t>
   </si>
@@ -665,9 +665,6 @@
   </si>
   <si>
     <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Register_Description'] = '…'</t>
-  </si>
-  <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Initial_Value'] = '…'</t>
   </si>
   <si>
     <t>hex number</t>
@@ -1250,6 +1247,9 @@
   </si>
   <si>
     <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config']['Ful_BitRange'] = []</t>
+  </si>
+  <si>
+    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Register_Address'] = '…'</t>
   </si>
 </sst>
 </file>
@@ -2834,8 +2834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2875,10 +2875,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2921,7 +2921,7 @@
         <v>147</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2929,7 +2929,7 @@
         <v>55</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2948,7 +2948,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2956,7 +2956,7 @@
         <v>135</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -2975,7 +2975,7 @@
         <v>27</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>74</v>
@@ -3005,8 +3005,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
-        <v>1.3111111111111111</v>
+      <c r="A19" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>64</v>
@@ -3029,30 +3029,30 @@
         <v>62</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>146</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>0.63194444444444442</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="C21" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="8" t="s">
         <v>212</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3069,7 +3069,7 @@
         <v>95</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3086,7 +3086,7 @@
         <v>93</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3103,7 +3103,7 @@
         <v>91</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
         <v>89</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3137,7 +3137,7 @@
         <v>87</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3154,7 +3154,7 @@
         <v>85</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3171,7 +3171,7 @@
         <v>83</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3188,7 +3188,7 @@
         <v>81</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3205,7 +3205,7 @@
         <v>79</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3222,7 +3222,7 @@
         <v>40</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3230,7 +3230,7 @@
         <v>27</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>121</v>
@@ -3260,8 +3260,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="33" x14ac:dyDescent="0.25">
-      <c r="A35" s="18">
-        <v>1.3111111111111111</v>
+      <c r="A35" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="B35" s="17" t="s">
         <v>64</v>
@@ -3284,30 +3284,30 @@
         <v>62</v>
       </c>
       <c r="C36" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="5" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>0.63055555555555554</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="C37" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="8" t="s">
         <v>229</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3324,7 +3324,7 @@
         <v>110</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3341,7 +3341,7 @@
         <v>108</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3358,7 +3358,7 @@
         <v>106</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3375,7 +3375,7 @@
         <v>104</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3392,7 +3392,7 @@
         <v>102</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>100</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3426,7 +3426,7 @@
         <v>98</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3443,7 +3443,7 @@
         <v>38</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -3500,10 +3500,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3921,8 +3921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P47" sqref="P47"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -3937,7 +3937,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="N4" t="s">
         <v>152</v>
@@ -3957,14 +3957,14 @@
         <v>0</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E7" s="33"/>
       <c r="F7" s="33"/>
       <c r="H7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P7" t="s">
         <v>152</v>
@@ -3984,7 +3984,7 @@
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
       <c r="H9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P9" t="s">
         <v>73</v>
@@ -3994,7 +3994,7 @@
       <c r="E10" s="33"/>
       <c r="F10" s="33"/>
       <c r="H10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P10" t="s">
         <v>155</v>
@@ -4004,7 +4004,7 @@
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
       <c r="H11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P11" s="30" t="s">
         <v>157</v>
@@ -4014,7 +4014,7 @@
       <c r="E12" s="33"/>
       <c r="F12" s="33"/>
       <c r="H12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P12" s="30" t="s">
         <v>157</v>
@@ -4024,7 +4024,7 @@
       <c r="E13" s="33"/>
       <c r="F13" s="33"/>
       <c r="H13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P13" s="30" t="s">
         <v>157</v>
@@ -4034,7 +4034,7 @@
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
       <c r="H14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="P14" s="34" t="s">
         <v>137</v>
@@ -4044,7 +4044,7 @@
       <c r="E15" s="33"/>
       <c r="F15" s="33"/>
       <c r="H15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P15" s="30" t="s">
         <v>157</v>
@@ -4054,7 +4054,7 @@
       <c r="E16" s="33"/>
       <c r="F16" s="33"/>
       <c r="H16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P16" s="30" t="s">
         <v>157</v>
@@ -4064,7 +4064,7 @@
       <c r="E17" s="33"/>
       <c r="F17" s="33"/>
       <c r="H17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P17" s="30" t="s">
         <v>157</v>
@@ -4074,7 +4074,7 @@
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="H18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P18" s="30" t="s">
         <v>157</v>
@@ -4084,10 +4084,10 @@
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
       <c r="H19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="P19" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
@@ -4096,7 +4096,7 @@
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E21" s="33"/>
       <c r="F21" s="32">
@@ -4113,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="35" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
@@ -4121,7 +4121,7 @@
       <c r="F23" s="33"/>
       <c r="G23" s="33"/>
       <c r="I23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S23" t="s">
         <v>152</v>
@@ -4143,7 +4143,7 @@
       <c r="F25" s="33"/>
       <c r="G25" s="33"/>
       <c r="I25" s="35" t="s">
-        <v>159</v>
+        <v>240</v>
       </c>
       <c r="J25" s="35"/>
       <c r="K25" s="35"/>
@@ -4155,7 +4155,7 @@
       <c r="Q25" s="35"/>
       <c r="R25" s="35"/>
       <c r="S25" s="35" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T25" s="35"/>
     </row>
@@ -4164,7 +4164,7 @@
       <c r="F26" s="33"/>
       <c r="G26" s="33"/>
       <c r="I26" s="35" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J26" s="35"/>
       <c r="K26" s="35"/>
@@ -4183,7 +4183,7 @@
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
       <c r="I27" s="35" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J27" s="35"/>
       <c r="K27" s="35"/>
@@ -4195,7 +4195,7 @@
       <c r="Q27" s="35"/>
       <c r="R27" s="35"/>
       <c r="S27" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T27" s="35"/>
     </row>
@@ -4204,7 +4204,7 @@
       <c r="F28" s="33"/>
       <c r="G28" s="33"/>
       <c r="I28" s="35" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="J28" s="35"/>
       <c r="K28" s="35"/>
@@ -4216,7 +4216,7 @@
       <c r="Q28" s="35"/>
       <c r="R28" s="35"/>
       <c r="S28" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T28" s="35"/>
     </row>
@@ -4225,7 +4225,7 @@
       <c r="F29" s="33"/>
       <c r="G29" s="33"/>
       <c r="I29" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J29" s="35"/>
       <c r="K29" s="35"/>
@@ -4237,7 +4237,7 @@
       <c r="Q29" s="35"/>
       <c r="R29" s="35"/>
       <c r="S29" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T29" s="35"/>
     </row>
@@ -4246,7 +4246,7 @@
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
       <c r="I30" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J30" s="35"/>
       <c r="K30" s="35"/>
@@ -4258,7 +4258,7 @@
       <c r="Q30" s="35"/>
       <c r="R30" s="35"/>
       <c r="S30" s="35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T30" s="35"/>
     </row>
@@ -4269,7 +4269,7 @@
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E32" s="33"/>
       <c r="F32" s="33"/>
@@ -4277,7 +4277,7 @@
         <v>1</v>
       </c>
       <c r="H32" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -4288,7 +4288,7 @@
         <v>0</v>
       </c>
       <c r="I33" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -4297,7 +4297,7 @@
       <c r="G34" s="33"/>
       <c r="H34" s="33"/>
       <c r="J34" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="V34" t="s">
         <v>152</v>
@@ -4309,7 +4309,7 @@
       <c r="G35" s="33"/>
       <c r="H35" s="33"/>
       <c r="J35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="V35" t="s">
         <v>152</v>
@@ -4321,10 +4321,10 @@
       <c r="G36" s="33"/>
       <c r="H36" s="33"/>
       <c r="J36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="V36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -4333,10 +4333,10 @@
       <c r="G37" s="33"/>
       <c r="H37" s="33"/>
       <c r="J37" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="V37" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -4347,7 +4347,7 @@
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E39" s="33"/>
       <c r="F39" s="33"/>
@@ -4356,7 +4356,7 @@
         <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
@@ -4365,7 +4365,7 @@
       <c r="G40" s="33"/>
       <c r="H40" s="33"/>
       <c r="J40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="W40" t="s">
         <v>155</v>
@@ -4377,10 +4377,10 @@
       <c r="G41" s="33"/>
       <c r="H41" s="33"/>
       <c r="J41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="W41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
@@ -4389,7 +4389,7 @@
       <c r="G42" s="33"/>
       <c r="H42" s="33"/>
       <c r="J42" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="W42" t="s">
         <v>155</v>
@@ -4401,10 +4401,10 @@
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
       <c r="J43" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="W43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -4415,7 +4415,7 @@
         <v>2</v>
       </c>
       <c r="I44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
@@ -4423,10 +4423,10 @@
       <c r="F45" s="33"/>
       <c r="G45" s="33"/>
       <c r="H45" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
@@ -4436,17 +4436,17 @@
         <v>2</v>
       </c>
       <c r="H46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="E47" s="33"/>
       <c r="F47" s="33"/>
       <c r="G47" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
@@ -4455,16 +4455,16 @@
         <v>2</v>
       </c>
       <c r="G48" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E49" s="33"/>
       <c r="F49" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.25">
@@ -4472,15 +4472,15 @@
         <v>2</v>
       </c>
       <c r="F50" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E51" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Resolve the generation error
</commit_message>
<xml_diff>
--- a/input/RegSpec_Org.xlsx
+++ b/input/RegSpec_Org.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\RegRTLGen\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\20.Project\3.Github\RegRTLGen\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="5" r:id="rId1"/>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="242">
   <si>
     <t>No</t>
   </si>
@@ -1249,13 +1249,35 @@
     <t>RegSpec[RegSpec_Example][Register_No_1][Register_Field_No_1]['Common_Config']['Ful_BitRange'] = []</t>
   </si>
   <si>
-    <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['Register_Address'] = '…'</t>
+    <r>
+      <t>RegSpec[RegSpec_Example][Register_No_1]['Common_Config']['</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>GenRegOffsetParam</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>'] = '…'</t>
+    </r>
+  </si>
+  <si>
+    <t>15:10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="13"/>
@@ -1997,19 +2019,19 @@
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>47</v>
       </c>
@@ -2017,7 +2039,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -2025,12 +2047,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>52</v>
       </c>
@@ -2049,17 +2071,17 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="4.78515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="10.640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.35546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2076,7 +2098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2093,7 +2115,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2128,15 +2150,15 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="3.35546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.2109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2147,7 +2169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2158,7 +2180,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="82.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="66" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2169,7 +2191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="49.5" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2199,272 +2221,272 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="20" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.88671875" style="20" customWidth="1"/>
-    <col min="4" max="256" width="9.109375" style="20"/>
-    <col min="257" max="257" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="69.88671875" style="20" customWidth="1"/>
-    <col min="260" max="512" width="9.109375" style="20"/>
-    <col min="513" max="513" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="514" max="514" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="515" max="515" width="69.88671875" style="20" customWidth="1"/>
-    <col min="516" max="768" width="9.109375" style="20"/>
-    <col min="769" max="769" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="770" max="770" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="771" max="771" width="69.88671875" style="20" customWidth="1"/>
-    <col min="772" max="1024" width="9.109375" style="20"/>
-    <col min="1025" max="1025" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1026" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="1027" max="1027" width="69.88671875" style="20" customWidth="1"/>
-    <col min="1028" max="1280" width="9.109375" style="20"/>
-    <col min="1281" max="1281" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1282" max="1282" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="1283" max="1283" width="69.88671875" style="20" customWidth="1"/>
-    <col min="1284" max="1536" width="9.109375" style="20"/>
-    <col min="1537" max="1537" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1538" max="1538" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="1539" max="1539" width="69.88671875" style="20" customWidth="1"/>
-    <col min="1540" max="1792" width="9.109375" style="20"/>
-    <col min="1793" max="1793" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="1794" max="1794" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="1795" max="1795" width="69.88671875" style="20" customWidth="1"/>
-    <col min="1796" max="2048" width="9.109375" style="20"/>
-    <col min="2049" max="2049" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2050" max="2050" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2051" max="2051" width="69.88671875" style="20" customWidth="1"/>
-    <col min="2052" max="2304" width="9.109375" style="20"/>
-    <col min="2305" max="2305" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2306" max="2306" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2307" max="2307" width="69.88671875" style="20" customWidth="1"/>
-    <col min="2308" max="2560" width="9.109375" style="20"/>
-    <col min="2561" max="2561" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2562" max="2562" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2563" max="2563" width="69.88671875" style="20" customWidth="1"/>
-    <col min="2564" max="2816" width="9.109375" style="20"/>
-    <col min="2817" max="2817" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="2818" max="2818" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="2819" max="2819" width="69.88671875" style="20" customWidth="1"/>
-    <col min="2820" max="3072" width="9.109375" style="20"/>
-    <col min="3073" max="3073" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3074" max="3074" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3075" max="3075" width="69.88671875" style="20" customWidth="1"/>
-    <col min="3076" max="3328" width="9.109375" style="20"/>
-    <col min="3329" max="3329" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3330" max="3330" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3331" max="3331" width="69.88671875" style="20" customWidth="1"/>
-    <col min="3332" max="3584" width="9.109375" style="20"/>
-    <col min="3585" max="3585" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3586" max="3586" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3587" max="3587" width="69.88671875" style="20" customWidth="1"/>
-    <col min="3588" max="3840" width="9.109375" style="20"/>
-    <col min="3841" max="3841" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="3842" max="3842" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3843" max="3843" width="69.88671875" style="20" customWidth="1"/>
-    <col min="3844" max="4096" width="9.109375" style="20"/>
-    <col min="4097" max="4097" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4098" max="4098" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4099" max="4099" width="69.88671875" style="20" customWidth="1"/>
-    <col min="4100" max="4352" width="9.109375" style="20"/>
-    <col min="4353" max="4353" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4354" max="4354" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4355" max="4355" width="69.88671875" style="20" customWidth="1"/>
-    <col min="4356" max="4608" width="9.109375" style="20"/>
-    <col min="4609" max="4609" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4610" max="4610" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4611" max="4611" width="69.88671875" style="20" customWidth="1"/>
-    <col min="4612" max="4864" width="9.109375" style="20"/>
-    <col min="4865" max="4865" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="4866" max="4866" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="4867" max="4867" width="69.88671875" style="20" customWidth="1"/>
-    <col min="4868" max="5120" width="9.109375" style="20"/>
-    <col min="5121" max="5121" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5122" max="5122" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5123" max="5123" width="69.88671875" style="20" customWidth="1"/>
-    <col min="5124" max="5376" width="9.109375" style="20"/>
-    <col min="5377" max="5377" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5378" max="5378" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5379" max="5379" width="69.88671875" style="20" customWidth="1"/>
-    <col min="5380" max="5632" width="9.109375" style="20"/>
-    <col min="5633" max="5633" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5634" max="5634" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5635" max="5635" width="69.88671875" style="20" customWidth="1"/>
-    <col min="5636" max="5888" width="9.109375" style="20"/>
-    <col min="5889" max="5889" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5890" max="5890" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="5891" max="5891" width="69.88671875" style="20" customWidth="1"/>
-    <col min="5892" max="6144" width="9.109375" style="20"/>
-    <col min="6145" max="6145" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6146" max="6146" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6147" max="6147" width="69.88671875" style="20" customWidth="1"/>
-    <col min="6148" max="6400" width="9.109375" style="20"/>
-    <col min="6401" max="6401" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6402" max="6402" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6403" max="6403" width="69.88671875" style="20" customWidth="1"/>
-    <col min="6404" max="6656" width="9.109375" style="20"/>
-    <col min="6657" max="6657" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6658" max="6658" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6659" max="6659" width="69.88671875" style="20" customWidth="1"/>
-    <col min="6660" max="6912" width="9.109375" style="20"/>
-    <col min="6913" max="6913" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="6914" max="6914" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="6915" max="6915" width="69.88671875" style="20" customWidth="1"/>
-    <col min="6916" max="7168" width="9.109375" style="20"/>
-    <col min="7169" max="7169" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7170" max="7170" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7171" max="7171" width="69.88671875" style="20" customWidth="1"/>
-    <col min="7172" max="7424" width="9.109375" style="20"/>
-    <col min="7425" max="7425" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7426" max="7426" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7427" max="7427" width="69.88671875" style="20" customWidth="1"/>
-    <col min="7428" max="7680" width="9.109375" style="20"/>
-    <col min="7681" max="7681" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7682" max="7682" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7683" max="7683" width="69.88671875" style="20" customWidth="1"/>
-    <col min="7684" max="7936" width="9.109375" style="20"/>
-    <col min="7937" max="7937" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="7938" max="7938" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="7939" max="7939" width="69.88671875" style="20" customWidth="1"/>
-    <col min="7940" max="8192" width="9.109375" style="20"/>
-    <col min="8193" max="8193" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8194" max="8194" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8195" max="8195" width="69.88671875" style="20" customWidth="1"/>
-    <col min="8196" max="8448" width="9.109375" style="20"/>
-    <col min="8449" max="8449" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8450" max="8450" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8451" max="8451" width="69.88671875" style="20" customWidth="1"/>
-    <col min="8452" max="8704" width="9.109375" style="20"/>
-    <col min="8705" max="8705" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8706" max="8706" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8707" max="8707" width="69.88671875" style="20" customWidth="1"/>
-    <col min="8708" max="8960" width="9.109375" style="20"/>
-    <col min="8961" max="8961" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="8962" max="8962" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="8963" max="8963" width="69.88671875" style="20" customWidth="1"/>
-    <col min="8964" max="9216" width="9.109375" style="20"/>
-    <col min="9217" max="9217" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9218" max="9218" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9219" max="9219" width="69.88671875" style="20" customWidth="1"/>
-    <col min="9220" max="9472" width="9.109375" style="20"/>
-    <col min="9473" max="9473" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9474" max="9474" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9475" max="9475" width="69.88671875" style="20" customWidth="1"/>
-    <col min="9476" max="9728" width="9.109375" style="20"/>
-    <col min="9729" max="9729" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9730" max="9730" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9731" max="9731" width="69.88671875" style="20" customWidth="1"/>
-    <col min="9732" max="9984" width="9.109375" style="20"/>
-    <col min="9985" max="9985" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="9986" max="9986" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="9987" max="9987" width="69.88671875" style="20" customWidth="1"/>
-    <col min="9988" max="10240" width="9.109375" style="20"/>
-    <col min="10241" max="10241" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10242" max="10242" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="10243" max="10243" width="69.88671875" style="20" customWidth="1"/>
-    <col min="10244" max="10496" width="9.109375" style="20"/>
-    <col min="10497" max="10497" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10498" max="10498" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="10499" max="10499" width="69.88671875" style="20" customWidth="1"/>
-    <col min="10500" max="10752" width="9.109375" style="20"/>
-    <col min="10753" max="10753" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="10754" max="10754" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="10755" max="10755" width="69.88671875" style="20" customWidth="1"/>
-    <col min="10756" max="11008" width="9.109375" style="20"/>
-    <col min="11009" max="11009" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11010" max="11010" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11011" max="11011" width="69.88671875" style="20" customWidth="1"/>
-    <col min="11012" max="11264" width="9.109375" style="20"/>
-    <col min="11265" max="11265" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11266" max="11266" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11267" max="11267" width="69.88671875" style="20" customWidth="1"/>
-    <col min="11268" max="11520" width="9.109375" style="20"/>
-    <col min="11521" max="11521" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11522" max="11522" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11523" max="11523" width="69.88671875" style="20" customWidth="1"/>
-    <col min="11524" max="11776" width="9.109375" style="20"/>
-    <col min="11777" max="11777" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="11778" max="11778" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="11779" max="11779" width="69.88671875" style="20" customWidth="1"/>
-    <col min="11780" max="12032" width="9.109375" style="20"/>
-    <col min="12033" max="12033" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12034" max="12034" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="12035" max="12035" width="69.88671875" style="20" customWidth="1"/>
-    <col min="12036" max="12288" width="9.109375" style="20"/>
-    <col min="12289" max="12289" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12290" max="12290" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="12291" max="12291" width="69.88671875" style="20" customWidth="1"/>
-    <col min="12292" max="12544" width="9.109375" style="20"/>
-    <col min="12545" max="12545" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12546" max="12546" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="12547" max="12547" width="69.88671875" style="20" customWidth="1"/>
-    <col min="12548" max="12800" width="9.109375" style="20"/>
-    <col min="12801" max="12801" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="12802" max="12802" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="12803" max="12803" width="69.88671875" style="20" customWidth="1"/>
-    <col min="12804" max="13056" width="9.109375" style="20"/>
-    <col min="13057" max="13057" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13058" max="13058" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13059" max="13059" width="69.88671875" style="20" customWidth="1"/>
-    <col min="13060" max="13312" width="9.109375" style="20"/>
-    <col min="13313" max="13313" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13314" max="13314" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13315" max="13315" width="69.88671875" style="20" customWidth="1"/>
-    <col min="13316" max="13568" width="9.109375" style="20"/>
-    <col min="13569" max="13569" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13570" max="13570" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13571" max="13571" width="69.88671875" style="20" customWidth="1"/>
-    <col min="13572" max="13824" width="9.109375" style="20"/>
-    <col min="13825" max="13825" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="13826" max="13826" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="13827" max="13827" width="69.88671875" style="20" customWidth="1"/>
-    <col min="13828" max="14080" width="9.109375" style="20"/>
-    <col min="14081" max="14081" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14082" max="14082" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="14083" max="14083" width="69.88671875" style="20" customWidth="1"/>
-    <col min="14084" max="14336" width="9.109375" style="20"/>
-    <col min="14337" max="14337" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14338" max="14338" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="14339" max="14339" width="69.88671875" style="20" customWidth="1"/>
-    <col min="14340" max="14592" width="9.109375" style="20"/>
-    <col min="14593" max="14593" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14594" max="14594" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="14595" max="14595" width="69.88671875" style="20" customWidth="1"/>
-    <col min="14596" max="14848" width="9.109375" style="20"/>
-    <col min="14849" max="14849" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="14850" max="14850" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="14851" max="14851" width="69.88671875" style="20" customWidth="1"/>
-    <col min="14852" max="15104" width="9.109375" style="20"/>
-    <col min="15105" max="15105" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15106" max="15106" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="15107" max="15107" width="69.88671875" style="20" customWidth="1"/>
-    <col min="15108" max="15360" width="9.109375" style="20"/>
-    <col min="15361" max="15361" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15362" max="15362" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="15363" max="15363" width="69.88671875" style="20" customWidth="1"/>
-    <col min="15364" max="15616" width="9.109375" style="20"/>
-    <col min="15617" max="15617" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15618" max="15618" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="15619" max="15619" width="69.88671875" style="20" customWidth="1"/>
-    <col min="15620" max="15872" width="9.109375" style="20"/>
-    <col min="15873" max="15873" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="15874" max="15874" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="15875" max="15875" width="69.88671875" style="20" customWidth="1"/>
-    <col min="15876" max="16128" width="9.109375" style="20"/>
-    <col min="16129" max="16129" width="4.88671875" style="20" bestFit="1" customWidth="1"/>
-    <col min="16130" max="16130" width="11.33203125" style="20" bestFit="1" customWidth="1"/>
-    <col min="16131" max="16131" width="69.88671875" style="20" customWidth="1"/>
-    <col min="16132" max="16384" width="9.109375" style="20"/>
+    <col min="1" max="1" width="4.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.85546875" style="20" customWidth="1"/>
+    <col min="4" max="256" width="9.140625" style="20"/>
+    <col min="257" max="257" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="69.85546875" style="20" customWidth="1"/>
+    <col min="260" max="512" width="9.140625" style="20"/>
+    <col min="513" max="513" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="514" max="514" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="515" max="515" width="69.85546875" style="20" customWidth="1"/>
+    <col min="516" max="768" width="9.140625" style="20"/>
+    <col min="769" max="769" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="770" max="770" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="771" max="771" width="69.85546875" style="20" customWidth="1"/>
+    <col min="772" max="1024" width="9.140625" style="20"/>
+    <col min="1025" max="1025" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1026" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1027" max="1027" width="69.85546875" style="20" customWidth="1"/>
+    <col min="1028" max="1280" width="9.140625" style="20"/>
+    <col min="1281" max="1281" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1282" max="1282" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1283" max="1283" width="69.85546875" style="20" customWidth="1"/>
+    <col min="1284" max="1536" width="9.140625" style="20"/>
+    <col min="1537" max="1537" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1538" max="1538" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1539" max="1539" width="69.85546875" style="20" customWidth="1"/>
+    <col min="1540" max="1792" width="9.140625" style="20"/>
+    <col min="1793" max="1793" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1794" max="1794" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="1795" max="1795" width="69.85546875" style="20" customWidth="1"/>
+    <col min="1796" max="2048" width="9.140625" style="20"/>
+    <col min="2049" max="2049" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2050" max="2050" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2051" max="2051" width="69.85546875" style="20" customWidth="1"/>
+    <col min="2052" max="2304" width="9.140625" style="20"/>
+    <col min="2305" max="2305" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2306" max="2306" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2307" max="2307" width="69.85546875" style="20" customWidth="1"/>
+    <col min="2308" max="2560" width="9.140625" style="20"/>
+    <col min="2561" max="2561" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2562" max="2562" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2563" max="2563" width="69.85546875" style="20" customWidth="1"/>
+    <col min="2564" max="2816" width="9.140625" style="20"/>
+    <col min="2817" max="2817" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2818" max="2818" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="2819" max="2819" width="69.85546875" style="20" customWidth="1"/>
+    <col min="2820" max="3072" width="9.140625" style="20"/>
+    <col min="3073" max="3073" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3074" max="3074" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3075" max="3075" width="69.85546875" style="20" customWidth="1"/>
+    <col min="3076" max="3328" width="9.140625" style="20"/>
+    <col min="3329" max="3329" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3330" max="3330" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3331" max="3331" width="69.85546875" style="20" customWidth="1"/>
+    <col min="3332" max="3584" width="9.140625" style="20"/>
+    <col min="3585" max="3585" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3586" max="3586" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3587" max="3587" width="69.85546875" style="20" customWidth="1"/>
+    <col min="3588" max="3840" width="9.140625" style="20"/>
+    <col min="3841" max="3841" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3842" max="3842" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="3843" max="3843" width="69.85546875" style="20" customWidth="1"/>
+    <col min="3844" max="4096" width="9.140625" style="20"/>
+    <col min="4097" max="4097" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4098" max="4098" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4099" max="4099" width="69.85546875" style="20" customWidth="1"/>
+    <col min="4100" max="4352" width="9.140625" style="20"/>
+    <col min="4353" max="4353" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4354" max="4354" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4355" max="4355" width="69.85546875" style="20" customWidth="1"/>
+    <col min="4356" max="4608" width="9.140625" style="20"/>
+    <col min="4609" max="4609" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4610" max="4610" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4611" max="4611" width="69.85546875" style="20" customWidth="1"/>
+    <col min="4612" max="4864" width="9.140625" style="20"/>
+    <col min="4865" max="4865" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4866" max="4866" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="4867" max="4867" width="69.85546875" style="20" customWidth="1"/>
+    <col min="4868" max="5120" width="9.140625" style="20"/>
+    <col min="5121" max="5121" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5122" max="5122" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5123" max="5123" width="69.85546875" style="20" customWidth="1"/>
+    <col min="5124" max="5376" width="9.140625" style="20"/>
+    <col min="5377" max="5377" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5378" max="5378" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5379" max="5379" width="69.85546875" style="20" customWidth="1"/>
+    <col min="5380" max="5632" width="9.140625" style="20"/>
+    <col min="5633" max="5633" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5634" max="5634" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5635" max="5635" width="69.85546875" style="20" customWidth="1"/>
+    <col min="5636" max="5888" width="9.140625" style="20"/>
+    <col min="5889" max="5889" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5890" max="5890" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="5891" max="5891" width="69.85546875" style="20" customWidth="1"/>
+    <col min="5892" max="6144" width="9.140625" style="20"/>
+    <col min="6145" max="6145" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6146" max="6146" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6147" max="6147" width="69.85546875" style="20" customWidth="1"/>
+    <col min="6148" max="6400" width="9.140625" style="20"/>
+    <col min="6401" max="6401" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6402" max="6402" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6403" max="6403" width="69.85546875" style="20" customWidth="1"/>
+    <col min="6404" max="6656" width="9.140625" style="20"/>
+    <col min="6657" max="6657" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6658" max="6658" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6659" max="6659" width="69.85546875" style="20" customWidth="1"/>
+    <col min="6660" max="6912" width="9.140625" style="20"/>
+    <col min="6913" max="6913" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6914" max="6914" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="6915" max="6915" width="69.85546875" style="20" customWidth="1"/>
+    <col min="6916" max="7168" width="9.140625" style="20"/>
+    <col min="7169" max="7169" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7170" max="7170" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7171" max="7171" width="69.85546875" style="20" customWidth="1"/>
+    <col min="7172" max="7424" width="9.140625" style="20"/>
+    <col min="7425" max="7425" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7426" max="7426" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7427" max="7427" width="69.85546875" style="20" customWidth="1"/>
+    <col min="7428" max="7680" width="9.140625" style="20"/>
+    <col min="7681" max="7681" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7682" max="7682" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7683" max="7683" width="69.85546875" style="20" customWidth="1"/>
+    <col min="7684" max="7936" width="9.140625" style="20"/>
+    <col min="7937" max="7937" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7938" max="7938" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="7939" max="7939" width="69.85546875" style="20" customWidth="1"/>
+    <col min="7940" max="8192" width="9.140625" style="20"/>
+    <col min="8193" max="8193" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8194" max="8194" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8195" max="8195" width="69.85546875" style="20" customWidth="1"/>
+    <col min="8196" max="8448" width="9.140625" style="20"/>
+    <col min="8449" max="8449" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8450" max="8450" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8451" max="8451" width="69.85546875" style="20" customWidth="1"/>
+    <col min="8452" max="8704" width="9.140625" style="20"/>
+    <col min="8705" max="8705" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8706" max="8706" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8707" max="8707" width="69.85546875" style="20" customWidth="1"/>
+    <col min="8708" max="8960" width="9.140625" style="20"/>
+    <col min="8961" max="8961" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8962" max="8962" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="8963" max="8963" width="69.85546875" style="20" customWidth="1"/>
+    <col min="8964" max="9216" width="9.140625" style="20"/>
+    <col min="9217" max="9217" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9218" max="9218" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9219" max="9219" width="69.85546875" style="20" customWidth="1"/>
+    <col min="9220" max="9472" width="9.140625" style="20"/>
+    <col min="9473" max="9473" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9474" max="9474" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9475" max="9475" width="69.85546875" style="20" customWidth="1"/>
+    <col min="9476" max="9728" width="9.140625" style="20"/>
+    <col min="9729" max="9729" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9730" max="9730" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9731" max="9731" width="69.85546875" style="20" customWidth="1"/>
+    <col min="9732" max="9984" width="9.140625" style="20"/>
+    <col min="9985" max="9985" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9986" max="9986" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="9987" max="9987" width="69.85546875" style="20" customWidth="1"/>
+    <col min="9988" max="10240" width="9.140625" style="20"/>
+    <col min="10241" max="10241" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10242" max="10242" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10243" max="10243" width="69.85546875" style="20" customWidth="1"/>
+    <col min="10244" max="10496" width="9.140625" style="20"/>
+    <col min="10497" max="10497" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10498" max="10498" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10499" max="10499" width="69.85546875" style="20" customWidth="1"/>
+    <col min="10500" max="10752" width="9.140625" style="20"/>
+    <col min="10753" max="10753" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10754" max="10754" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="10755" max="10755" width="69.85546875" style="20" customWidth="1"/>
+    <col min="10756" max="11008" width="9.140625" style="20"/>
+    <col min="11009" max="11009" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11010" max="11010" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11011" max="11011" width="69.85546875" style="20" customWidth="1"/>
+    <col min="11012" max="11264" width="9.140625" style="20"/>
+    <col min="11265" max="11265" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11266" max="11266" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11267" max="11267" width="69.85546875" style="20" customWidth="1"/>
+    <col min="11268" max="11520" width="9.140625" style="20"/>
+    <col min="11521" max="11521" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11522" max="11522" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11523" max="11523" width="69.85546875" style="20" customWidth="1"/>
+    <col min="11524" max="11776" width="9.140625" style="20"/>
+    <col min="11777" max="11777" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11778" max="11778" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="11779" max="11779" width="69.85546875" style="20" customWidth="1"/>
+    <col min="11780" max="12032" width="9.140625" style="20"/>
+    <col min="12033" max="12033" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12034" max="12034" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12035" max="12035" width="69.85546875" style="20" customWidth="1"/>
+    <col min="12036" max="12288" width="9.140625" style="20"/>
+    <col min="12289" max="12289" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12290" max="12290" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12291" max="12291" width="69.85546875" style="20" customWidth="1"/>
+    <col min="12292" max="12544" width="9.140625" style="20"/>
+    <col min="12545" max="12545" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12546" max="12546" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12547" max="12547" width="69.85546875" style="20" customWidth="1"/>
+    <col min="12548" max="12800" width="9.140625" style="20"/>
+    <col min="12801" max="12801" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12802" max="12802" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="12803" max="12803" width="69.85546875" style="20" customWidth="1"/>
+    <col min="12804" max="13056" width="9.140625" style="20"/>
+    <col min="13057" max="13057" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13058" max="13058" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13059" max="13059" width="69.85546875" style="20" customWidth="1"/>
+    <col min="13060" max="13312" width="9.140625" style="20"/>
+    <col min="13313" max="13313" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13314" max="13314" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13315" max="13315" width="69.85546875" style="20" customWidth="1"/>
+    <col min="13316" max="13568" width="9.140625" style="20"/>
+    <col min="13569" max="13569" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13570" max="13570" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13571" max="13571" width="69.85546875" style="20" customWidth="1"/>
+    <col min="13572" max="13824" width="9.140625" style="20"/>
+    <col min="13825" max="13825" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13826" max="13826" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="13827" max="13827" width="69.85546875" style="20" customWidth="1"/>
+    <col min="13828" max="14080" width="9.140625" style="20"/>
+    <col min="14081" max="14081" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14082" max="14082" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14083" max="14083" width="69.85546875" style="20" customWidth="1"/>
+    <col min="14084" max="14336" width="9.140625" style="20"/>
+    <col min="14337" max="14337" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14338" max="14338" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14339" max="14339" width="69.85546875" style="20" customWidth="1"/>
+    <col min="14340" max="14592" width="9.140625" style="20"/>
+    <col min="14593" max="14593" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14594" max="14594" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14595" max="14595" width="69.85546875" style="20" customWidth="1"/>
+    <col min="14596" max="14848" width="9.140625" style="20"/>
+    <col min="14849" max="14849" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14850" max="14850" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="14851" max="14851" width="69.85546875" style="20" customWidth="1"/>
+    <col min="14852" max="15104" width="9.140625" style="20"/>
+    <col min="15105" max="15105" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15106" max="15106" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15107" max="15107" width="69.85546875" style="20" customWidth="1"/>
+    <col min="15108" max="15360" width="9.140625" style="20"/>
+    <col min="15361" max="15361" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15362" max="15362" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15363" max="15363" width="69.85546875" style="20" customWidth="1"/>
+    <col min="15364" max="15616" width="9.140625" style="20"/>
+    <col min="15617" max="15617" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15618" max="15618" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15619" max="15619" width="69.85546875" style="20" customWidth="1"/>
+    <col min="15620" max="15872" width="9.140625" style="20"/>
+    <col min="15873" max="15873" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15874" max="15874" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="15875" max="15875" width="69.85546875" style="20" customWidth="1"/>
+    <col min="15876" max="16128" width="9.140625" style="20"/>
+    <col min="16129" max="16129" width="4.85546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="16130" max="16130" width="11.35546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="16131" max="16131" width="69.85546875" style="20" customWidth="1"/>
+    <col min="16132" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>77</v>
       </c>
@@ -2475,7 +2497,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A3" s="21">
         <v>1</v>
       </c>
@@ -2486,7 +2508,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A4" s="21">
         <v>2</v>
       </c>
@@ -2497,7 +2519,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A5" s="21">
         <v>3</v>
       </c>
@@ -2508,7 +2530,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A6" s="21">
         <v>4</v>
       </c>
@@ -2519,7 +2541,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A7" s="21">
         <v>5</v>
       </c>
@@ -2530,7 +2552,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A8" s="21">
         <v>6</v>
       </c>
@@ -2541,7 +2563,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A9" s="21">
         <v>7</v>
       </c>
@@ -2552,7 +2574,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A10" s="21">
         <v>8</v>
       </c>
@@ -2563,7 +2585,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A11" s="21">
         <v>9</v>
       </c>
@@ -2574,7 +2596,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A12" s="21">
         <v>10</v>
       </c>
@@ -2585,7 +2607,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="21">
         <v>11</v>
       </c>
@@ -2596,7 +2618,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="21">
         <v>12</v>
       </c>
@@ -2607,7 +2629,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="21">
         <v>13</v>
       </c>
@@ -2618,7 +2640,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="21">
         <v>14</v>
       </c>
@@ -2629,7 +2651,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="21">
         <v>15</v>
       </c>
@@ -2640,7 +2662,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="21">
         <v>16</v>
       </c>
@@ -2651,7 +2673,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="21">
         <v>17</v>
       </c>
@@ -2662,7 +2684,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="21">
         <v>18</v>
       </c>
@@ -2673,12 +2695,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="19" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="27" t="s">
         <v>77</v>
       </c>
@@ -2689,7 +2711,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A24" s="21">
         <v>1</v>
       </c>
@@ -2700,7 +2722,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A25" s="21">
         <v>2</v>
       </c>
@@ -2711,7 +2733,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A26" s="21">
         <v>3</v>
       </c>
@@ -2722,7 +2744,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="40.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="40" x14ac:dyDescent="0.35">
       <c r="A27" s="21">
         <v>4</v>
       </c>
@@ -2747,25 +2769,25 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="11"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2776,7 +2798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -2787,7 +2809,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -2798,7 +2820,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>21</v>
@@ -2807,7 +2829,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>10</v>
@@ -2816,7 +2838,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2834,27 +2856,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.2109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.78515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.35546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
@@ -2865,7 +2887,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -2873,7 +2895,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>168</v>
       </c>
@@ -2881,7 +2903,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
@@ -2889,7 +2911,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -2897,7 +2919,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>69</v>
       </c>
@@ -2908,7 +2930,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>70</v>
       </c>
@@ -2916,7 +2938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>147</v>
       </c>
@@ -2924,7 +2946,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
@@ -2932,7 +2954,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>136</v>
       </c>
@@ -2943,7 +2965,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
@@ -2951,7 +2973,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>135</v>
       </c>
@@ -2959,7 +2981,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
@@ -2970,7 +2992,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>27</v>
       </c>
@@ -2987,7 +3009,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -3004,7 +3026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>63</v>
       </c>
@@ -3021,7 +3043,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>59</v>
       </c>
@@ -3038,9 +3060,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
-        <v>143</v>
+        <v>241</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>209</v>
@@ -3055,7 +3077,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>9</v>
       </c>
@@ -3072,7 +3094,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>8</v>
       </c>
@@ -3089,7 +3111,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>7</v>
       </c>
@@ -3106,7 +3128,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>6</v>
       </c>
@@ -3123,7 +3145,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>5</v>
       </c>
@@ -3140,7 +3162,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>4</v>
       </c>
@@ -3157,7 +3179,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>3</v>
       </c>
@@ -3174,7 +3196,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>2</v>
       </c>
@@ -3191,7 +3213,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>1</v>
       </c>
@@ -3208,7 +3230,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>0</v>
       </c>
@@ -3225,7 +3247,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
         <v>27</v>
       </c>
@@ -3239,10 +3261,10 @@
         <v>122</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
@@ -3259,7 +3281,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="33" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
         <v>63</v>
       </c>
@@ -3276,7 +3298,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>59</v>
       </c>
@@ -3293,7 +3315,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="26" t="s">
         <v>143</v>
       </c>
@@ -3310,7 +3332,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>7</v>
       </c>
@@ -3327,7 +3349,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>6</v>
       </c>
@@ -3344,7 +3366,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>5</v>
       </c>
@@ -3361,7 +3383,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>4</v>
       </c>
@@ -3378,7 +3400,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>3</v>
       </c>
@@ -3395,7 +3417,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>2</v>
       </c>
@@ -3412,7 +3434,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>1</v>
       </c>
@@ -3429,7 +3451,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>0</v>
       </c>
@@ -3463,23 +3485,23 @@
       <selection activeCell="A3" sqref="A3:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="16.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.2109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.78515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.35546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>27</v>
       </c>
@@ -3490,7 +3512,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
@@ -3498,7 +3520,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>168</v>
       </c>
@@ -3506,7 +3528,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>53</v>
       </c>
@@ -3514,7 +3536,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -3522,7 +3544,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>69</v>
       </c>
@@ -3533,7 +3555,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>70</v>
       </c>
@@ -3541,7 +3563,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>147</v>
       </c>
@@ -3549,7 +3571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
@@ -3557,7 +3579,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>136</v>
       </c>
@@ -3568,7 +3590,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>56</v>
       </c>
@@ -3576,7 +3598,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>135</v>
       </c>
@@ -3584,7 +3606,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>34</v>
       </c>
@@ -3595,7 +3617,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
         <v>27</v>
       </c>
@@ -3612,7 +3634,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>35</v>
       </c>
@@ -3629,7 +3651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="33" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>63</v>
       </c>
@@ -3646,7 +3668,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>59</v>
       </c>
@@ -3663,7 +3685,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="49.5" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>15</v>
       </c>
@@ -3680,7 +3702,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="33" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>58</v>
       </c>
@@ -3697,7 +3719,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="49.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="49.5" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>0</v>
       </c>
@@ -3714,7 +3736,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
         <v>27</v>
       </c>
@@ -3731,7 +3753,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
@@ -3748,7 +3770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="s">
         <v>63</v>
       </c>
@@ -3763,7 +3785,7 @@
       </c>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>59</v>
       </c>
@@ -3778,7 +3800,7 @@
       </c>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="26" t="s">
         <v>128</v>
       </c>
@@ -3793,7 +3815,7 @@
       </c>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
         <v>126</v>
       </c>
@@ -3808,7 +3830,7 @@
       </c>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>0</v>
       </c>
@@ -3840,12 +3862,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>139</v>
       </c>
@@ -3856,7 +3878,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>141</v>
       </c>
@@ -3867,7 +3889,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C4">
         <v>1</v>
       </c>
@@ -3875,7 +3897,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C5">
         <v>2</v>
       </c>
@@ -3883,7 +3905,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C6">
         <v>3</v>
       </c>
@@ -3891,7 +3913,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>148</v>
       </c>
@@ -3902,12 +3924,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C8" s="30" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>150</v>
       </c>
@@ -3921,18 +3943,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:W52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E4" s="31">
         <v>0</v>
       </c>
@@ -3943,7 +3965,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="5" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E5" s="32">
         <v>1</v>
       </c>
@@ -3951,7 +3973,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E6" s="33"/>
       <c r="F6" s="31">
         <v>0</v>
@@ -3960,7 +3982,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E7" s="33"/>
       <c r="F7" s="33"/>
       <c r="H7" t="s">
@@ -3970,7 +3992,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E8" s="33"/>
       <c r="F8" s="33"/>
       <c r="H8" t="s">
@@ -3980,7 +4002,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E9" s="33"/>
       <c r="F9" s="33"/>
       <c r="H9" t="s">
@@ -3990,7 +4012,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E10" s="33"/>
       <c r="F10" s="33"/>
       <c r="H10" t="s">
@@ -4000,7 +4022,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
       <c r="H11" t="s">
@@ -4010,7 +4032,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E12" s="33"/>
       <c r="F12" s="33"/>
       <c r="H12" t="s">
@@ -4020,7 +4042,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E13" s="33"/>
       <c r="F13" s="33"/>
       <c r="H13" t="s">
@@ -4030,7 +4052,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="14" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
       <c r="H14" t="s">
@@ -4040,7 +4062,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E15" s="33"/>
       <c r="F15" s="33"/>
       <c r="H15" t="s">
@@ -4050,7 +4072,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="16" spans="5:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:16" x14ac:dyDescent="0.35">
       <c r="E16" s="33"/>
       <c r="F16" s="33"/>
       <c r="H16" t="s">
@@ -4060,7 +4082,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E17" s="33"/>
       <c r="F17" s="33"/>
       <c r="H17" t="s">
@@ -4070,7 +4092,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
       <c r="H18" t="s">
@@ -4080,7 +4102,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
       <c r="H19" t="s">
@@ -4090,11 +4112,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E20" s="33"/>
       <c r="F20" s="33"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>188</v>
       </c>
@@ -4106,7 +4128,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E22" s="33"/>
       <c r="F22" s="33"/>
       <c r="G22" s="31">
@@ -4116,7 +4138,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E23" s="33"/>
       <c r="F23" s="33"/>
       <c r="G23" s="33"/>
@@ -4127,7 +4149,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E24" s="33"/>
       <c r="F24" s="33"/>
       <c r="G24" s="33"/>
@@ -4138,7 +4160,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E25" s="33"/>
       <c r="F25" s="33"/>
       <c r="G25" s="33"/>
@@ -4159,7 +4181,7 @@
       </c>
       <c r="T25" s="35"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E26" s="33"/>
       <c r="F26" s="33"/>
       <c r="G26" s="33"/>
@@ -4178,7 +4200,7 @@
       <c r="S26" s="35"/>
       <c r="T26" s="35"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E27" s="33"/>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
@@ -4199,7 +4221,7 @@
       </c>
       <c r="T27" s="35"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E28" s="33"/>
       <c r="F28" s="33"/>
       <c r="G28" s="33"/>
@@ -4220,7 +4242,7 @@
       </c>
       <c r="T28" s="35"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E29" s="33"/>
       <c r="F29" s="33"/>
       <c r="G29" s="33"/>
@@ -4241,7 +4263,7 @@
       </c>
       <c r="T29" s="35"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E30" s="33"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
@@ -4262,12 +4284,12 @@
       </c>
       <c r="T30" s="35"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
       <c r="E31" s="33"/>
       <c r="F31" s="33"/>
       <c r="G31" s="33"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>189</v>
       </c>
@@ -4280,7 +4302,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E33" s="33"/>
       <c r="F33" s="33"/>
       <c r="G33" s="33"/>
@@ -4291,7 +4313,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E34" s="33"/>
       <c r="F34" s="33"/>
       <c r="G34" s="33"/>
@@ -4303,7 +4325,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E35" s="33"/>
       <c r="F35" s="33"/>
       <c r="G35" s="33"/>
@@ -4315,7 +4337,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E36" s="33"/>
       <c r="F36" s="33"/>
       <c r="G36" s="33"/>
@@ -4327,7 +4349,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E37" s="33"/>
       <c r="F37" s="33"/>
       <c r="G37" s="33"/>
@@ -4339,13 +4361,13 @@
         <v>170</v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E38" s="33"/>
       <c r="F38" s="33"/>
       <c r="G38" s="33"/>
       <c r="H38" s="33"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>190</v>
       </c>
@@ -4359,7 +4381,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E40" s="33"/>
       <c r="F40" s="33"/>
       <c r="G40" s="33"/>
@@ -4371,7 +4393,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E41" s="33"/>
       <c r="F41" s="33"/>
       <c r="G41" s="33"/>
@@ -4383,7 +4405,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E42" s="33"/>
       <c r="F42" s="33"/>
       <c r="G42" s="33"/>
@@ -4395,7 +4417,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E43" s="33"/>
       <c r="F43" s="33"/>
       <c r="G43" s="33"/>
@@ -4407,7 +4429,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E44" s="33"/>
       <c r="F44" s="33"/>
       <c r="G44" s="33"/>
@@ -4418,7 +4440,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E45" s="33"/>
       <c r="F45" s="33"/>
       <c r="G45" s="33"/>
@@ -4429,7 +4451,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E46" s="33"/>
       <c r="F46" s="33"/>
       <c r="G46" s="32">
@@ -4439,7 +4461,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E47" s="33"/>
       <c r="F47" s="33"/>
       <c r="G47" s="32" t="s">
@@ -4449,7 +4471,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="E48" s="33"/>
       <c r="F48" s="32">
         <v>2</v>
@@ -4458,7 +4480,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E49" s="33"/>
       <c r="F49" s="32" t="s">
         <v>161</v>
@@ -4467,7 +4489,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E50" s="32">
         <v>2</v>
       </c>
@@ -4475,7 +4497,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E51" s="32" t="s">
         <v>161</v>
       </c>
@@ -4483,7 +4505,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E52" s="33"/>
     </row>
   </sheetData>

</xml_diff>